<commit_message>
Backup QR Scanner data - 2025-12-27T08:29:33.771Z - Cache Bust: 1766824173771
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766225219729_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766225219729_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1982,9 +1982,269 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>201850</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C80" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D80" t="str">
+        <v>13:21:52</v>
+      </c>
+      <c r="E80" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F80" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>201694</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C81" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D81" t="str">
+        <v>13:21:56</v>
+      </c>
+      <c r="E81" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F81" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>201790</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C82" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D82" t="str">
+        <v>13:21:58</v>
+      </c>
+      <c r="E82" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F82" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>201488</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C83" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D83" t="str">
+        <v>13:22:13</v>
+      </c>
+      <c r="E83" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F83" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>201676</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C84" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D84" t="str">
+        <v>13:22:16</v>
+      </c>
+      <c r="E84" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F84" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>201619</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C85" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D85" t="str">
+        <v>13:22:19</v>
+      </c>
+      <c r="E85" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F85" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>201667</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C86" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D86" t="str">
+        <v>13:22:22</v>
+      </c>
+      <c r="E86" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F86" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>201675</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C87" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D87" t="str">
+        <v>13:22:24</v>
+      </c>
+      <c r="E87" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F87" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>201681</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C88" t="str">
+        <v>20/12/2025</v>
+      </c>
+      <c r="D88" t="str">
+        <v>13:22:29</v>
+      </c>
+      <c r="E88" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F88" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>201561</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C89" t="str">
+        <v>27/12/2025</v>
+      </c>
+      <c r="D89" t="str">
+        <v>10:23:07</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F89" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>212033</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C90" t="str">
+        <v>27/12/2025</v>
+      </c>
+      <c r="D90" t="str">
+        <v>10:23:47</v>
+      </c>
+      <c r="E90" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F90" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>201987</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C91" t="str">
+        <v>27/12/2025</v>
+      </c>
+      <c r="D91" t="str">
+        <v>10:24:26</v>
+      </c>
+      <c r="E91" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F91" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>201498</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C92" t="str">
+        <v>27/12/2025</v>
+      </c>
+      <c r="D92" t="str">
+        <v>10:24:38</v>
+      </c>
+      <c r="E92" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F92" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F79"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F92"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>